<commit_message>
Edit MatchProbe to reduce running time
</commit_message>
<xml_diff>
--- a/data-raw/Data_summaryforpackage.xlsx
+++ b/data-raw/Data_summaryforpackage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xutaowang/Desktop/curatedTBData/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F40D50-B076-1F41-B667-C1B04D4DFB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A369B8DC-3FFC-3D4E-87C1-E176BD775C87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="460" windowWidth="32760" windowHeight="16380" xr2:uid="{B39B7F83-2537-C248-AAB4-54D9192DC10F}"/>
   </bookViews>
@@ -355,9 +355,6 @@
     <t>1-15</t>
   </si>
   <si>
-    <t>Sputum culture, TST, QFT-GIT</t>
-  </si>
-  <si>
     <t>GSE62147</t>
   </si>
   <si>
@@ -715,6 +712,9 @@
   <si>
     <t xml:space="preserve">
 Ex vivo blood samples analysed at diagnosis and after 1, 2, 4 and 26 weeks of treatment (Total Measure=135).</t>
+  </si>
+  <si>
+    <t>Sputum culture, TST, IGRA(QFT-GIT)</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1288,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1324,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>7</v>
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>8</v>
@@ -1342,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="69" customHeight="1">
@@ -1365,7 +1365,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H2">
         <v>6</v>
@@ -1381,15 +1381,15 @@
         <v>21</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="70" customHeight="1">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1417,15 +1417,15 @@
         <v>9</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="63" customHeight="1">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -1450,15 +1450,15 @@
         <v>27</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1492,7 +1492,7 @@
         <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="34">
@@ -1515,7 +1515,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="H6">
         <v>9</v>
@@ -1531,12 +1531,12 @@
         <v>27</v>
       </c>
       <c r="N6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="119">
       <c r="A7" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>93</v>
@@ -1554,7 +1554,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13">
@@ -1569,15 +1569,15 @@
         <v>334</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="119">
       <c r="A8" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1595,7 +1595,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I8">
         <v>104</v>
@@ -1608,15 +1608,15 @@
         <v>144</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="119">
       <c r="A9" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -1632,7 +1632,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H9">
         <v>100</v>
@@ -1645,15 +1645,15 @@
         <v>138</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="51">
       <c r="A10" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -1687,12 +1687,12 @@
         <v>33</v>
       </c>
       <c r="N10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="51">
       <c r="A11" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -1726,12 +1726,12 @@
         <v>44</v>
       </c>
       <c r="N11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="62" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1762,15 +1762,15 @@
         <v>31</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="49" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1807,30 +1807,30 @@
         <v>96</v>
       </c>
       <c r="N13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="49" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I14">
         <v>16</v>
@@ -1844,12 +1844,12 @@
       </c>
       <c r="M14" s="4"/>
       <c r="N14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="49" customHeight="1">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
@@ -1864,7 +1864,7 @@
         <v>69</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H15">
         <v>16</v>
@@ -1878,30 +1878,30 @@
       </c>
       <c r="M15" s="4"/>
       <c r="N15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="49" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I16">
         <v>21</v>
@@ -1914,18 +1914,18 @@
         <v>51</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="49" customHeight="1">
       <c r="A17" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
@@ -1934,10 +1934,10 @@
         <v>19</v>
       </c>
       <c r="E17" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="H17">
         <v>32</v>
@@ -1950,10 +1950,10 @@
         <v>48</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1976,7 +1976,7 @@
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H18">
         <v>12</v>
@@ -2015,7 +2015,7 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H19">
         <v>16</v>
@@ -2051,7 +2051,7 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I20">
         <v>31</v>
@@ -2090,7 +2090,7 @@
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H21">
         <v>12</v>
@@ -2120,13 +2120,13 @@
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22">
         <v>12</v>
@@ -2162,7 +2162,7 @@
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H23">
         <v>81</v>
@@ -2175,7 +2175,7 @@
         <v>274</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N23" t="s">
         <v>97</v>
@@ -2214,7 +2214,7 @@
         <v>36</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N24" t="s">
         <v>97</v>
@@ -2240,7 +2240,7 @@
         <v>69</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I25">
         <v>14</v>
@@ -2256,7 +2256,7 @@
         <v>157</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N25" t="s">
         <v>97</v>
@@ -2270,7 +2270,7 @@
         <v>65</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -2282,7 +2282,7 @@
         <v>69</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I26">
         <v>54</v>
@@ -2298,7 +2298,7 @@
         <v>334</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N26" t="s">
         <v>97</v>
@@ -2321,10 +2321,10 @@
         <v>20</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I27">
         <v>35</v>
@@ -2337,7 +2337,7 @@
         <v>50</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N27" t="s">
         <v>97</v>
@@ -2360,7 +2360,7 @@
         <v>77</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H28">
         <v>22</v>
@@ -2373,7 +2373,7 @@
         <v>43</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N28" t="s">
         <v>97</v>
@@ -2399,7 +2399,7 @@
         <v>69</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I29">
         <v>167</v>
@@ -2415,7 +2415,7 @@
         <v>537</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N29" t="s">
         <v>97</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="30" spans="1:14" ht="113" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
@@ -2637,7 +2637,7 @@
         <v>7</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N35" t="s">
         <v>97</v>
@@ -2679,7 +2679,7 @@
         <v>15</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N36" t="s">
         <v>97</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="37" spans="1:14" ht="34">
       <c r="A37" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
         <v>65</v>
@@ -2699,10 +2699,10 @@
         <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G37" t="s">
         <v>23</v>
@@ -2721,7 +2721,7 @@
         <v>110</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N37" t="s">
         <v>97</v>
@@ -2763,7 +2763,7 @@
         <v>108</v>
       </c>
       <c r="N38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="17">
@@ -2799,10 +2799,10 @@
         <v>44</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="34">
@@ -2835,10 +2835,10 @@
         <v>21</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="85">
@@ -2858,7 +2858,7 @@
         <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H41">
         <v>76</v>
@@ -2871,10 +2871,10 @@
         <v>189</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="51">
@@ -2907,24 +2907,24 @@
         <v>72</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N42" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="51">
       <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
         <v>104</v>
-      </c>
-      <c r="B43" t="s">
-        <v>105</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H43">
         <v>13</v>
@@ -2941,12 +2941,12 @@
       </c>
       <c r="M43" s="4"/>
       <c r="N43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="51">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
         <v>50</v>
@@ -2961,7 +2961,7 @@
         <v>15</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J44">
         <v>26</v>
@@ -2971,10 +2971,10 @@
         <v>26</v>
       </c>
       <c r="M44" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -3025,15 +3025,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
         <v>141</v>
-      </c>
-      <c r="B1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17">
       <c r="A2" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>63</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="3" spans="1:2" ht="17">
       <c r="A3" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>64</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="4" spans="1:2" ht="17">
       <c r="A4" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>74</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="5" spans="1:2" ht="17">
       <c r="A5" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>29</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="6" spans="1:2" ht="17">
       <c r="A6" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>30</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="7" spans="1:2" ht="17">
       <c r="A7" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>34</v>
@@ -3081,15 +3081,15 @@
     </row>
     <row r="8" spans="1:2" ht="17">
       <c r="A8" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>144</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17">
       <c r="A9" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>36</v>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="10" spans="1:2" ht="17">
       <c r="A10" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>37</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="11" spans="1:2" ht="17">
       <c r="A11" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>10</v>
@@ -3113,31 +3113,31 @@
     </row>
     <row r="12" spans="1:2" ht="17">
       <c r="A12" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17">
       <c r="A13" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17">
       <c r="A14" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17">
       <c r="A15" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>70</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="16" spans="1:2" ht="17">
       <c r="A16" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>49</v>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="17" spans="1:2" ht="17">
       <c r="A17" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>47</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="18" spans="1:2" ht="17">
       <c r="A18" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>80</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="19" spans="1:2" ht="17">
       <c r="A19" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>81</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="20" spans="1:2" ht="17">
       <c r="A20" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>82</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="21" spans="1:2" ht="17">
       <c r="A21" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>83</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="22" spans="1:2" ht="17">
       <c r="A22" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>84</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="23" spans="1:2" ht="17">
       <c r="A23" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>85</v>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="24" spans="1:2" ht="17">
       <c r="A24" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>75</v>
@@ -3217,7 +3217,7 @@
     </row>
     <row r="25" spans="1:2" ht="17">
       <c r="A25" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>61</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="26" spans="1:2" ht="17">
       <c r="A26" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>51</v>
@@ -3233,23 +3233,23 @@
     </row>
     <row r="27" spans="1:2" ht="17">
       <c r="A27" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17">
       <c r="A28" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17">
       <c r="A29" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>53</v>
@@ -3257,23 +3257,23 @@
     </row>
     <row r="30" spans="1:2" ht="17">
       <c r="A30" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>153</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17">
       <c r="A31" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17">
       <c r="A32" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>76</v>
@@ -3281,39 +3281,39 @@
     </row>
     <row r="33" spans="1:2" ht="17">
       <c r="A33" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17">
       <c r="A34" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17">
       <c r="A35" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17">
       <c r="A36" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>80</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>81</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>82</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>83</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>84</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>85</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>29</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>30</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>34</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>35</v>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>36</v>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>37</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49" s="21" t="s">
         <v>98</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>74</v>
@@ -3425,50 +3425,50 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="21" t="s">
         <v>159</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17">
       <c r="A54" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" s="27" t="s">
         <v>161</v>
-      </c>
-      <c r="B54" s="27" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>